<commit_message>
Fix a few issues
</commit_message>
<xml_diff>
--- a/examsLinksTemplate.xlsx
+++ b/examsLinksTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gtelem/pgit/DB-Exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C38C4-231A-0140-A358-95D954EAF61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A1F943-6998-7942-8081-4C7CD1691535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="12780" windowWidth="25760" windowHeight="16660" xr2:uid="{DE768112-1DBF-FA44-842F-AC23B3CAB8F3}"/>
   </bookViews>
@@ -265,148 +265,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -578,6 +450,70 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor auto="1"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -592,16 +528,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FB41E9E-1896-4D45-BE18-DD028BC190D6}" name="Table1" displayName="Table1" ref="A15:G95" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1FB41E9E-1896-4D45-BE18-DD028BC190D6}" name="Table1" displayName="Table1" ref="A15:G95" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A15:G95" xr:uid="{1FB41E9E-1896-4D45-BE18-DD028BC190D6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{03287FFF-3492-5446-8529-0F7E88456FBE}" name="שנה" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{F9760AE5-3262-7E47-B397-01FCB1F714E4}" name="סמסטר" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{8C1AB8FD-7ABC-5D46-AD77-28F23167F1EB}" name="מועד" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{128214DE-59B7-0F4A-A9C4-D575CE974E58}" name="לינק" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{415BEE98-392E-C941-835D-FFF5EF09882B}" name="בוצע?" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{D3EBBBD7-B485-9640-A7D9-BF3E6B267657}" name="פתרון" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{31095883-383B-5C46-B362-69F5F5D7D85D}" name="הערות" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{03287FFF-3492-5446-8529-0F7E88456FBE}" name="שנה" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F9760AE5-3262-7E47-B397-01FCB1F714E4}" name="סמסטר" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8C1AB8FD-7ABC-5D46-AD77-28F23167F1EB}" name="מועד" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{128214DE-59B7-0F4A-A9C4-D575CE974E58}" name="לינק" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{415BEE98-392E-C941-835D-FFF5EF09882B}" name="בוצע?" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D3EBBBD7-B485-9640-A7D9-BF3E6B267657}" name="פתרון" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{31095883-383B-5C46-B362-69F5F5D7D85D}" name="הערות" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,7 +843,7 @@
   <dimension ref="A2:I95"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -921,20 +857,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -996,20 +932,20 @@
         <f ca="1">YEAR(TODAY())-10</f>
         <v>2012</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f ca="1">YEAR(TODAY())-5</f>
         <v>2017</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -2195,19 +2131,19 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1000">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>ISNUMBER(A16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2221,27 +2157,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F9 A11:F1048576 A10:B10 D10:F10">
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
       <formula>AND(XFD1 = "חסר", B1 = "/")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>A1="/"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>A1="חסר"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>A1="-"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>A1="v"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
       <formula>A1="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
       <formula>ISNUMBER(XFA9)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>